<commit_message>
Completed new driver config implementation. Updated drivers implementation. Updated unit tests for selenium. Refactored main execution loop.
</commit_message>
<xml_diff>
--- a/examples/demo/simple_demo.xlsx
+++ b/examples/demo/simple_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desjajo\Documents\_TASS\tass-ssat-framework\tass-ssat\examples\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{3C7045F4-0745-47C0-AB07-F502CFFF8A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E045C9D-F894-43CC-AF43-881785E385EB}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{3C7045F4-0745-47C0-AB07-F502CFFF8A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75D5E0D-71D1-4E0B-AF30-32176FED363C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.6"/>
@@ -727,7 +727,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
@@ -801,7 +801,7 @@
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
@@ -1307,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA85F721-ED58-498A-9F1C-B499A899A1A4}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Updated examples and converter for Logger implementation.
</commit_message>
<xml_diff>
--- a/examples/demo/simple_demo.xlsx
+++ b/examples/demo/simple_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t xml:space="preserve">V2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_path:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./log2</t>
   </si>
   <si>
     <t xml:space="preserve">test suites:</t>
@@ -625,7 +631,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,37 +657,43 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -715,13 +727,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,34 +746,34 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -799,198 +811,198 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1027,258 +1039,258 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12" s="3"/>
       <c r="I12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3"/>
       <c r="K13" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1314,49 +1326,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1392,52 +1404,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1473,49 +1485,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1551,47 +1563,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200 feature improve logger (#203)
* Initial commit for logging implementation.

* Updated logger handler for customization.

* Renamed default config function

* Updated examples and converter for Logger implementation.
</commit_message>
<xml_diff>
--- a/examples/demo/simple_demo.xlsx
+++ b/examples/demo/simple_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t xml:space="preserve">V2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_path:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./log2</t>
   </si>
   <si>
     <t xml:space="preserve">test suites:</t>
@@ -625,7 +631,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,37 +657,43 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -715,13 +727,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,34 +746,34 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -799,198 +811,198 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1027,258 +1039,258 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12" s="3"/>
       <c r="I12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3"/>
       <c r="K13" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1314,49 +1326,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1392,52 +1404,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1473,49 +1485,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1551,47 +1563,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tass converter mobile implementation.
</commit_message>
<xml_diff>
--- a/examples/demo/simple_demo.xlsx
+++ b/examples/demo/simple_demo.xlsx
@@ -15,7 +15,8 @@
     <sheet name="chrome001" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="chrome002" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="ffox001" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="ffox002" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="android" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="ffox002" sheetId="9" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="92">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -65,27 +66,33 @@
     <t xml:space="preserve">reporters:</t>
   </si>
   <si>
+    <t xml:space="preserve">drivers:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chrome001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uuid-tc-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ffox002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">android001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr100102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Demo 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">browsers:</t>
   </si>
   <si>
-    <t xml:space="preserve">chrome001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">others:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uuid-tc-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffox002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tr100102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple Demo 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">chrome002</t>
   </si>
   <si>
@@ -276,6 +283,27 @@
   </si>
   <si>
     <t xml:space="preserve">explicit_wait,30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mb_uuid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">platform_name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key[,value]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appium:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--testing1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--testing,more</t>
   </si>
 </sst>
 </file>
@@ -286,7 +314,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -307,6 +335,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -358,12 +391,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,7 +412,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,10 +668,10 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -657,10 +694,10 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -697,7 +734,11 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -720,20 +761,20 @@
       <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,10 +799,10 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>14</v>
@@ -773,7 +814,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -800,209 +841,209 @@
       <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="40.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="29.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="I7" s="2" t="s">
-        <v>54</v>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1027,270 +1068,270 @@
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="38.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="28.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="38.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>63</v>
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="I12" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="I7" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="I12" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="K13" s="2" t="s">
-        <v>66</v>
+      <c r="G13" s="4"/>
+      <c r="K13" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1356,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
@@ -1326,49 +1367,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1434,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.42"/>
@@ -1404,52 +1445,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1471,10 +1512,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
@@ -1485,49 +1526,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>70</v>
+      <c r="B2" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1546,13 +1587,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
@@ -1563,47 +1604,137 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>